<commit_message>
Testing: before I drive myself crazy.
</commit_message>
<xml_diff>
--- a/testSheets/sum.xlsx
+++ b/testSheets/sum.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\git\Excel-Function-Visualizer\testSheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28680" windowHeight="10005"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21615" windowHeight="6750"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -339,7 +335,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -357,6 +353,10 @@
       <c r="A2">
         <v>2</v>
       </c>
+      <c r="C2">
+        <f>SUM(A:A)</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">

</xml_diff>